<commit_message>
Insertion and other bibliographies
</commit_message>
<xml_diff>
--- a/Bibliography/BibliographyResearch.xlsx
+++ b/Bibliography/BibliographyResearch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\BipedProject\Bibliography\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7527090-1C91-4291-B609-AD81EE9AE4AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35165DF5-2592-4CFC-99BC-AB5D7B7C76E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t xml:space="preserve">Topic </t>
   </si>
@@ -90,6 +90,21 @@
 1) Calculation of algebraic constraint vector and constraint Jacobian matrix for arbitary foot shape
 2) Explanation of the only one differentiation constraint vector for algebraic equation solution 
 3) Methodology for foot shape selection based on human-like ankle trajectory </t>
+  </si>
+  <si>
+    <t>JBE21.pdf</t>
+  </si>
+  <si>
+    <t>22.01.22</t>
+  </si>
+  <si>
+    <t>In the biped walking model is completely investigated. Here you can find
+1)  Walking phases and events description
+2) Model structure and the parameters
+3) Gait function definition
+4) Gait stability definition
+5) Nominal model for opimal stability
+6) Effect of the parameter variations and conclutions</t>
   </si>
 </sst>
 </file>
@@ -344,6 +359,50 @@
         <a:xfrm>
           <a:off x="6741459" y="3316941"/>
           <a:ext cx="1707471" cy="986118"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>143435</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1792941</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1681585</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA1B6C7F-BF85-6740-8C8D-52293B58C3A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6750424" y="4831976"/>
+          <a:ext cx="1640541" cy="1538150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -620,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,6 +764,20 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7" s="13"/>
       <c r="D7" s="2"/>
@@ -720,9 +793,10 @@
     <hyperlink ref="F3" r:id="rId1" display="Consept/Knees/icra22.pdf" xr:uid="{75F98B0C-0984-4874-BC3B-096D937F87CA}"/>
     <hyperlink ref="F2" r:id="rId2" display="Consept/Knees/IROS22.pdf" xr:uid="{F85D353C-FDDE-414F-BAC2-16A8829CF34C}"/>
     <hyperlink ref="F4" r:id="rId3" display="Consept/NoKnees/ICRA20a.pdf" xr:uid="{174A8F63-5FDC-48A0-AE80-216F13BA6812}"/>
+    <hyperlink ref="F5" r:id="rId4" display="Consept/NoKnees/JBE21.pdf" xr:uid="{E99D45FA-A644-4099-AC49-E717FFD759E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Smyrli and simatos thesis write down
</commit_message>
<xml_diff>
--- a/Bibliography/BibliographyResearch.xlsx
+++ b/Bibliography/BibliographyResearch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\BipedProject\Bibliography\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35165DF5-2592-4CFC-99BC-AB5D7B7C76E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93B62CC-CC8E-4A2F-8A16-AB8C2D242526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t xml:space="preserve">Topic </t>
   </si>
@@ -105,6 +105,46 @@
 4) Gait stability definition
 5) Nominal model for opimal stability
 6) Effect of the parameter variations and conclutions</t>
+  </si>
+  <si>
+    <t>Smyrli_thesis_final.pdf</t>
+  </si>
+  <si>
+    <t>22.01.25</t>
+  </si>
+  <si>
+    <t>Biped robot conscept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In this thesis you can find: 
+1) Insertion of constraints using lagrange multipliers
+2) Parameterization analisys + analysis of the parameters effect
+3) Introduction to poincare illustration
+4) Model equations
+5)  Phase alteration conditions
+6)  Control of the robot and fully actuated model based system in order to determine wich of the DoFs are important to have actuation
+7) Insertion non linear p-v terms in the control
+</t>
+  </si>
+  <si>
+    <t>Vasileiou_Thesis_2019.pdf</t>
+  </si>
+  <si>
+    <t>Vasileiou Christos</t>
+  </si>
+  <si>
+    <t>Biped robot manufacturing</t>
+  </si>
+  <si>
+    <t>In this thesis you can find
+1) Dimension scaling analysis
+2)  Contact modeling, Friction modeling (stribeck model etc.), Stress and dynamic loading theory
+3) Adams modeling theory 
+4) Design specifications and design methods
+5) Loading profiles extraction
+6) Robastness study (k,b, μ, L deviations) of the model using Adams
+7) Manufacturing methods and subsystem validation
+8) Experimental setup description</t>
   </si>
 </sst>
 </file>
@@ -175,7 +215,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -214,6 +254,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -403,6 +444,50 @@
         <a:xfrm>
           <a:off x="6750424" y="4831976"/>
           <a:ext cx="1640541" cy="1538150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>107579</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>457201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1835761</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1882588</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{733F6F24-3346-4DB6-093F-BB86D1D89A18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6705603" y="6974542"/>
+          <a:ext cx="1728182" cy="1425387"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -677,20 +762,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.88671875" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.21875" style="6" customWidth="1"/>
     <col min="3" max="3" width="39.21875" customWidth="1"/>
     <col min="4" max="4" width="19.109375" customWidth="1"/>
     <col min="5" max="5" width="28" style="11" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="28.21875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -765,6 +850,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
@@ -778,15 +866,261 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="13"/>
-      <c r="D7" s="2"/>
-      <c r="F7" s="3"/>
+    <row r="6" spans="1:6" ht="195" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="193.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="14"/>
       <c r="D9" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="14"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="14"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="14"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C20" s="14"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C21" s="14"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C22" s="14"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C23" s="14"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C24" s="14"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C29" s="14"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C31" s="14"/>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" s="14"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" s="14"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" s="14"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C37" s="14"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C38" s="14"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C39" s="14"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C40" s="14"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C41" s="14"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C42" s="14"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C43" s="14"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C44" s="14"/>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C45" s="14"/>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C46" s="14"/>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C47" s="14"/>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C48" s="14"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="14"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C50" s="14"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C51" s="14"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C52" s="14"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C53" s="14"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C54" s="14"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C55" s="14"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C56" s="14"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C57" s="14"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C58" s="14"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C59" s="14"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C60" s="14"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C61" s="14"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C62" s="14"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C63" s="14"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C64" s="14"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C65" s="14"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C66" s="14"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C67" s="14"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C68" s="14"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C69" s="14"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C70" s="14"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C71" s="14"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C72" s="14"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C73" s="14"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C74" s="14"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C75" s="14"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C76" s="14"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C77" s="14"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C78" s="14"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C79" s="14"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C80" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -794,9 +1128,11 @@
     <hyperlink ref="F2" r:id="rId2" display="Consept/Knees/IROS22.pdf" xr:uid="{F85D353C-FDDE-414F-BAC2-16A8829CF34C}"/>
     <hyperlink ref="F4" r:id="rId3" display="Consept/NoKnees/ICRA20a.pdf" xr:uid="{174A8F63-5FDC-48A0-AE80-216F13BA6812}"/>
     <hyperlink ref="F5" r:id="rId4" display="Consept/NoKnees/JBE21.pdf" xr:uid="{E99D45FA-A644-4099-AC49-E717FFD759E2}"/>
+    <hyperlink ref="F6" r:id="rId5" display="Consept/NoKnees/Smyrli_thesis_final.pdf" xr:uid="{18718150-0A3D-4F8B-990C-F7D85497D9BD}"/>
+    <hyperlink ref="F7" r:id="rId6" display="Consept/NoKnees/Vasileiou_Thesis_2019.pdf" xr:uid="{42DB3B71-B4CF-498E-A846-5EACFC5F9B67}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId5"/>
-  <drawing r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId7"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Insertion of manufacturing solutions from bibliogrphy
</commit_message>
<xml_diff>
--- a/Bibliography/BibliographyResearch.xlsx
+++ b/Bibliography/BibliographyResearch.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\BipedProject\Bibliography\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A1A9B9-F2C3-4A72-92C4-B2A8D684A75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07078751-8852-4F75-839C-3EB9EDBD7734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bibliography" sheetId="1" r:id="rId1"/>
     <sheet name="Byped robot names" sheetId="3" r:id="rId2"/>
-    <sheet name="Keywords" sheetId="4" r:id="rId3"/>
+    <sheet name="Actuators" sheetId="4" r:id="rId3"/>
+    <sheet name="Foot design" sheetId="5" r:id="rId4"/>
+    <sheet name="Joints" sheetId="6" r:id="rId5"/>
+    <sheet name="Other manufacturing ideas" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t xml:space="preserve">Topic </t>
   </si>
@@ -83,9 +86,6 @@
   </si>
   <si>
     <t>Optimal foot shape study</t>
-  </si>
-  <si>
-    <t>`</t>
   </si>
   <si>
     <t xml:space="preserve">This paper introduces a methodology for arbitary foot shape generation in the passive walking dynamics
@@ -161,16 +161,10 @@
     <t>The Cornell Passive Biped</t>
   </si>
   <si>
-    <t>McGeer'ss Capstone Design</t>
-  </si>
-  <si>
     <t>Jerry Pratt's tow - dimensional walking robot</t>
   </si>
   <si>
     <t xml:space="preserve">Spring Flamingo </t>
-  </si>
-  <si>
-    <t>Dynamically controled motion</t>
   </si>
   <si>
     <t>3D Biped with knees and arms</t>
@@ -190,6 +184,38 @@
 2)  Lateral - swinging arms to stabilize side-to-side lean.
 3) Collisional indeterminacy rejection using hinged arcs (Soft heel design)  (This design can be modified for our application using as spring - rubber) 
 </t>
+  </si>
+  <si>
+    <t>22.01.27</t>
+  </si>
+  <si>
+    <t>McGeer's walker by Garcia</t>
+  </si>
+  <si>
+    <t>2D Design with hip and knees</t>
+  </si>
+  <si>
+    <t>Martijn Wisse</t>
+  </si>
+  <si>
+    <t>WisseBookMikeDesign.pdf</t>
+  </si>
+  <si>
+    <t>In this book you can find: 
+1) The testing no knees machine. (Intresting that the foot shapes are connected with screws
+2) Foot  design with switch (Allows to the controller to adapt ot the actual step time by resgistering the exact instant of heel strike
+3) We notice rectangular cross section in order the cables to pass through them
+4) Insertion of actuator requirment  (the actuators should not interfer with the passie swinging motion of the legs
+5)</t>
+  </si>
+  <si>
+    <t>Actuator type</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Geared motor</t>
   </si>
 </sst>
 </file>
@@ -268,7 +294,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -300,6 +325,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -629,6 +657,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>80682</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>62753</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>911654</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1425389</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CA81577-3A48-703C-4092-46523966722E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7234517" y="13070541"/>
+          <a:ext cx="830972" cy="1362636"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1079608</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>167127</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2188030</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1358046</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{272766FC-5E2F-ED4A-4E60-C7EEE67BF010}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8242408" y="13175556"/>
+          <a:ext cx="1108422" cy="1190919"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -895,27 +1011,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" style="5" customWidth="1"/>
     <col min="3" max="3" width="39.21875" customWidth="1"/>
     <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="28" style="11" customWidth="1"/>
-    <col min="6" max="6" width="30.77734375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.5546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="30.77734375" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -927,7 +1043,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -935,16 +1051,16 @@
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -952,16 +1068,16 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -969,305 +1085,465 @@
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>17</v>
+      <c r="C4" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>18</v>
+      <c r="F5" s="11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="195" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>21</v>
+      <c r="F6" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="193.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>28</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="3" t="s">
         <v>25</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="121.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="7" t="s">
+    </row>
+    <row r="9" spans="1:6" ht="126" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="14"/>
-      <c r="D9" t="s">
-        <v>16</v>
+      <c r="C9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="14"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C11" s="14"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="14"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="14"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="14"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="14"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="14"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" s="14"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C18" s="14"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C19" s="14"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C20" s="14"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C21" s="14"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C22" s="14"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C23" s="14"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C24" s="14"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C25" s="14"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C26" s="14"/>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C27" s="14"/>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C28" s="14"/>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C29" s="14"/>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C30" s="14"/>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C31" s="14"/>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C32" s="14"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="14"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" s="14"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C35" s="14"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="14"/>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="14"/>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="14"/>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C39" s="14"/>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C40" s="14"/>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C41" s="14"/>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C42" s="14"/>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C43" s="14"/>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C44" s="14"/>
-    </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C45" s="14"/>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C46" s="14"/>
-    </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C47" s="14"/>
-    </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C48" s="14"/>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C49" s="14"/>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C50" s="14"/>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C51" s="14"/>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C52" s="14"/>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C53" s="14"/>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C54" s="14"/>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C55" s="14"/>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C56" s="14"/>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C57" s="14"/>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C58" s="14"/>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C59" s="14"/>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C60" s="14"/>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C61" s="14"/>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C62" s="14"/>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C63" s="14"/>
-    </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C64" s="14"/>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C65" s="14"/>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C66" s="14"/>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C67" s="14"/>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C68" s="14"/>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C69" s="14"/>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C70" s="14"/>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C71" s="14"/>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C72" s="14"/>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C73" s="14"/>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C74" s="14"/>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C75" s="14"/>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C76" s="14"/>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C77" s="14"/>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C78" s="14"/>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C79" s="14"/>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C80" s="14"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" s="13"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="13"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" s="13"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="13"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21" s="13"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22" s="13"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C23" s="13"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C24" s="13"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C25" s="13"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C26" s="13"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C27" s="13"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C28" s="13"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C29" s="13"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C30" s="13"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C31" s="13"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C32" s="13"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C33" s="13"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C34" s="13"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C35" s="13"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C36" s="13"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C37" s="13"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C38" s="13"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C39" s="13"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C40" s="13"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C41" s="13"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C42" s="13"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C43" s="13"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C44" s="13"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C45" s="13"/>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C46" s="13"/>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C47" s="13"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C48" s="13"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C49" s="13"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C50" s="13"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C51" s="13"/>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C52" s="13"/>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C53" s="13"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C54" s="13"/>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C55" s="13"/>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C56" s="13"/>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C57" s="13"/>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C58" s="13"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C59" s="13"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C60" s="13"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C61" s="13"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C62" s="13"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C63" s="13"/>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C64" s="13"/>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C65" s="13"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C66" s="13"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C67" s="13"/>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C68" s="13"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C69" s="13"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C70" s="13"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C71" s="13"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C72" s="13"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C73" s="13"/>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C74" s="13"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C75" s="13"/>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C76" s="13"/>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C77" s="13"/>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C78" s="13"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C79" s="13"/>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C80" s="13"/>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D90" s="2"/>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D91" s="2"/>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D92" s="2"/>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D93" s="2"/>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D97" s="2"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D99" s="2"/>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D100" s="2"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D101" s="2"/>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D102" s="2"/>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D103" s="2"/>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D104" s="2"/>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D106" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1278,10 +1554,11 @@
     <hyperlink ref="F6" r:id="rId5" display="Consept/NoKnees/Smyrli_thesis_final.pdf" xr:uid="{18718150-0A3D-4F8B-990C-F7D85497D9BD}"/>
     <hyperlink ref="F7" r:id="rId6" display="Consept/NoKnees/Vasileiou_Thesis_2019.pdf" xr:uid="{42DB3B71-B4CF-498E-A846-5EACFC5F9B67}"/>
     <hyperlink ref="F8" r:id="rId7" display="Manufacturers/CollinsRuinaPassiveLegsKnees.pdf" xr:uid="{E03437DA-8456-4E3D-A8B2-249AE9844B57}"/>
+    <hyperlink ref="F9" r:id="rId8" display="Manufacturers/WisseBookMikeDesign.pdf" xr:uid="{6C7A0374-5A96-4F7A-A122-2AA6BCDAE8E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId8"/>
-  <drawing r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId9"/>
+  <drawing r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -1290,7 +1567,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1300,37 +1577,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1340,23 +1617,1906 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FEDA881-ECA0-4B5D-A1E8-7BBE47D7D9F9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C378"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
+    <row r="1" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="14"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="14"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="14"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="14"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="14"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="14"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="14"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="14"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="14"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="14"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="14"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="14"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="14"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="14"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="14"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="14"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="14"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="14"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="14"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="14"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="14"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="14"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="14"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="14"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="14"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="14"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="14"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="14"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="14"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="14"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="14"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="14"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="14"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="14"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="14"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="14"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="14"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="14"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="14"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="14"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="14"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="14"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="14"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="14"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="14"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="14"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="14"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="14"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="9"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="14"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="14"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="14"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="9"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="14"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="9"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="14"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="14"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="9"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="14"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="14"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="9"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="14"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="14"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="9"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="14"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="9"/>
+      <c r="B77" s="9"/>
+      <c r="C77" s="14"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="9"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="14"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="14"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="9"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="14"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="9"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="14"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="9"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="14"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="9"/>
+      <c r="B83" s="9"/>
+      <c r="C83" s="14"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="9"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="14"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="9"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="14"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="9"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="14"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="9"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="14"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="9"/>
+      <c r="B88" s="9"/>
+      <c r="C88" s="14"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="9"/>
+      <c r="B89" s="9"/>
+      <c r="C89" s="14"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="9"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="14"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="9"/>
+      <c r="B91" s="9"/>
+      <c r="C91" s="14"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="9"/>
+      <c r="B92" s="9"/>
+      <c r="C92" s="14"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="9"/>
+      <c r="B93" s="9"/>
+      <c r="C93" s="14"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="9"/>
+      <c r="B94" s="9"/>
+      <c r="C94" s="14"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="9"/>
+      <c r="B95" s="9"/>
+      <c r="C95" s="14"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="9"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="14"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="9"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="14"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" s="9"/>
+      <c r="B98" s="9"/>
+      <c r="C98" s="14"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" s="9"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="14"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" s="9"/>
+      <c r="B100" s="9"/>
+      <c r="C100" s="14"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" s="9"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="14"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" s="9"/>
+      <c r="B102" s="9"/>
+      <c r="C102" s="14"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" s="9"/>
+      <c r="B103" s="9"/>
+      <c r="C103" s="14"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" s="9"/>
+      <c r="B104" s="9"/>
+      <c r="C104" s="14"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" s="9"/>
+      <c r="B105" s="9"/>
+      <c r="C105" s="14"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" s="9"/>
+      <c r="B106" s="9"/>
+      <c r="C106" s="14"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="9"/>
+      <c r="B107" s="9"/>
+      <c r="C107" s="14"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="9"/>
+      <c r="B108" s="9"/>
+      <c r="C108" s="14"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="9"/>
+      <c r="B109" s="9"/>
+      <c r="C109" s="14"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="9"/>
+      <c r="B110" s="9"/>
+      <c r="C110" s="14"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="9"/>
+      <c r="B111" s="9"/>
+      <c r="C111" s="14"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="9"/>
+      <c r="B112" s="9"/>
+      <c r="C112" s="14"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="9"/>
+      <c r="B113" s="9"/>
+      <c r="C113" s="14"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="9"/>
+      <c r="B114" s="9"/>
+      <c r="C114" s="14"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="9"/>
+      <c r="B115" s="9"/>
+      <c r="C115" s="14"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="9"/>
+      <c r="B116" s="9"/>
+      <c r="C116" s="14"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="9"/>
+      <c r="B117" s="9"/>
+      <c r="C117" s="14"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="9"/>
+      <c r="B118" s="9"/>
+      <c r="C118" s="14"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="9"/>
+      <c r="B119" s="9"/>
+      <c r="C119" s="14"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="9"/>
+      <c r="B120" s="9"/>
+      <c r="C120" s="14"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="9"/>
+      <c r="B121" s="9"/>
+      <c r="C121" s="14"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="9"/>
+      <c r="B122" s="9"/>
+      <c r="C122" s="14"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="9"/>
+      <c r="B123" s="9"/>
+      <c r="C123" s="14"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="9"/>
+      <c r="B124" s="9"/>
+      <c r="C124" s="14"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="9"/>
+      <c r="B125" s="9"/>
+      <c r="C125" s="14"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" s="9"/>
+      <c r="B126" s="9"/>
+      <c r="C126" s="14"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" s="9"/>
+      <c r="B127" s="9"/>
+      <c r="C127" s="14"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" s="9"/>
+      <c r="B128" s="9"/>
+      <c r="C128" s="14"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="9"/>
+      <c r="B129" s="9"/>
+      <c r="C129" s="14"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="9"/>
+      <c r="B130" s="9"/>
+      <c r="C130" s="14"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="9"/>
+      <c r="B131" s="9"/>
+      <c r="C131" s="14"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="9"/>
+      <c r="B132" s="9"/>
+      <c r="C132" s="14"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" s="9"/>
+      <c r="B133" s="9"/>
+      <c r="C133" s="14"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" s="9"/>
+      <c r="B134" s="9"/>
+      <c r="C134" s="14"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="9"/>
+      <c r="B135" s="9"/>
+      <c r="C135" s="14"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" s="9"/>
+      <c r="B136" s="9"/>
+      <c r="C136" s="14"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" s="9"/>
+      <c r="B137" s="9"/>
+      <c r="C137" s="14"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" s="9"/>
+      <c r="B138" s="9"/>
+      <c r="C138" s="14"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" s="9"/>
+      <c r="B139" s="9"/>
+      <c r="C139" s="14"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" s="9"/>
+      <c r="B140" s="9"/>
+      <c r="C140" s="14"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" s="9"/>
+      <c r="B141" s="9"/>
+      <c r="C141" s="14"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" s="9"/>
+      <c r="B142" s="9"/>
+      <c r="C142" s="14"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" s="9"/>
+      <c r="B143" s="9"/>
+      <c r="C143" s="14"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" s="9"/>
+      <c r="B144" s="9"/>
+      <c r="C144" s="14"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" s="9"/>
+      <c r="B145" s="9"/>
+      <c r="C145" s="14"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" s="9"/>
+      <c r="B146" s="9"/>
+      <c r="C146" s="14"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" s="9"/>
+      <c r="B147" s="9"/>
+      <c r="C147" s="14"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" s="9"/>
+      <c r="B148" s="9"/>
+      <c r="C148" s="14"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" s="9"/>
+      <c r="B149" s="9"/>
+      <c r="C149" s="14"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" s="9"/>
+      <c r="B150" s="9"/>
+      <c r="C150" s="14"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151" s="9"/>
+      <c r="B151" s="9"/>
+      <c r="C151" s="14"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152" s="9"/>
+      <c r="B152" s="9"/>
+      <c r="C152" s="14"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A153" s="9"/>
+      <c r="B153" s="9"/>
+      <c r="C153" s="14"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A154" s="9"/>
+      <c r="B154" s="9"/>
+      <c r="C154" s="14"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A155" s="9"/>
+      <c r="B155" s="9"/>
+      <c r="C155" s="14"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A156" s="9"/>
+      <c r="B156" s="9"/>
+      <c r="C156" s="14"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A157" s="9"/>
+      <c r="B157" s="9"/>
+      <c r="C157" s="14"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A158" s="9"/>
+      <c r="B158" s="9"/>
+      <c r="C158" s="14"/>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A159" s="9"/>
+      <c r="B159" s="9"/>
+      <c r="C159" s="14"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A160" s="9"/>
+      <c r="B160" s="9"/>
+      <c r="C160" s="14"/>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A161" s="9"/>
+      <c r="B161" s="9"/>
+      <c r="C161" s="14"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A162" s="9"/>
+      <c r="B162" s="9"/>
+      <c r="C162" s="14"/>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A163" s="9"/>
+      <c r="B163" s="9"/>
+      <c r="C163" s="14"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A164" s="9"/>
+      <c r="B164" s="9"/>
+      <c r="C164" s="14"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A165" s="9"/>
+      <c r="B165" s="9"/>
+      <c r="C165" s="14"/>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166" s="9"/>
+      <c r="B166" s="9"/>
+      <c r="C166" s="14"/>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A167" s="9"/>
+      <c r="B167" s="9"/>
+      <c r="C167" s="14"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A168" s="9"/>
+      <c r="B168" s="9"/>
+      <c r="C168" s="14"/>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A169" s="9"/>
+      <c r="B169" s="9"/>
+      <c r="C169" s="14"/>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A170" s="9"/>
+      <c r="B170" s="9"/>
+      <c r="C170" s="14"/>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A171" s="9"/>
+      <c r="B171" s="9"/>
+      <c r="C171" s="14"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A172" s="9"/>
+      <c r="B172" s="9"/>
+      <c r="C172" s="14"/>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A173" s="9"/>
+      <c r="B173" s="9"/>
+      <c r="C173" s="14"/>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A174" s="9"/>
+      <c r="B174" s="9"/>
+      <c r="C174" s="14"/>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A175" s="9"/>
+      <c r="B175" s="9"/>
+      <c r="C175" s="14"/>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A176" s="9"/>
+      <c r="B176" s="9"/>
+      <c r="C176" s="14"/>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A177" s="9"/>
+      <c r="B177" s="9"/>
+      <c r="C177" s="14"/>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A178" s="9"/>
+      <c r="B178" s="9"/>
+      <c r="C178" s="14"/>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A179" s="9"/>
+      <c r="B179" s="9"/>
+      <c r="C179" s="14"/>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A180" s="9"/>
+      <c r="B180" s="9"/>
+      <c r="C180" s="14"/>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A181" s="9"/>
+      <c r="B181" s="9"/>
+      <c r="C181" s="14"/>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A182" s="9"/>
+      <c r="B182" s="9"/>
+      <c r="C182" s="14"/>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A183" s="9"/>
+      <c r="B183" s="9"/>
+      <c r="C183" s="14"/>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A184" s="9"/>
+      <c r="B184" s="9"/>
+      <c r="C184" s="14"/>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A185" s="9"/>
+      <c r="B185" s="9"/>
+      <c r="C185" s="14"/>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A186" s="9"/>
+      <c r="B186" s="9"/>
+      <c r="C186" s="14"/>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A187" s="9"/>
+      <c r="B187" s="9"/>
+      <c r="C187" s="14"/>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A188" s="9"/>
+      <c r="B188" s="9"/>
+      <c r="C188" s="14"/>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A189" s="9"/>
+      <c r="B189" s="9"/>
+      <c r="C189" s="14"/>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A190" s="9"/>
+      <c r="B190" s="9"/>
+      <c r="C190" s="14"/>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A191" s="9"/>
+      <c r="B191" s="9"/>
+      <c r="C191" s="14"/>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A192" s="9"/>
+      <c r="B192" s="9"/>
+      <c r="C192" s="14"/>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A193" s="9"/>
+      <c r="B193" s="9"/>
+      <c r="C193" s="14"/>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A194" s="9"/>
+      <c r="B194" s="9"/>
+      <c r="C194" s="14"/>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A195" s="9"/>
+      <c r="B195" s="9"/>
+      <c r="C195" s="14"/>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A196" s="9"/>
+      <c r="B196" s="9"/>
+      <c r="C196" s="14"/>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A197" s="9"/>
+      <c r="B197" s="9"/>
+      <c r="C197" s="14"/>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A198" s="9"/>
+      <c r="B198" s="9"/>
+      <c r="C198" s="14"/>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A199" s="9"/>
+      <c r="B199" s="9"/>
+      <c r="C199" s="14"/>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A200" s="9"/>
+      <c r="B200" s="9"/>
+      <c r="C200" s="14"/>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A201" s="9"/>
+      <c r="B201" s="9"/>
+      <c r="C201" s="14"/>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A202" s="9"/>
+      <c r="B202" s="9"/>
+      <c r="C202" s="14"/>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A203" s="9"/>
+      <c r="B203" s="9"/>
+      <c r="C203" s="14"/>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A204" s="9"/>
+      <c r="B204" s="9"/>
+      <c r="C204" s="14"/>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A205" s="9"/>
+      <c r="B205" s="9"/>
+      <c r="C205" s="14"/>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A206" s="9"/>
+      <c r="B206" s="9"/>
+      <c r="C206" s="14"/>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A207" s="9"/>
+      <c r="B207" s="9"/>
+      <c r="C207" s="14"/>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A208" s="9"/>
+      <c r="B208" s="9"/>
+      <c r="C208" s="14"/>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A209" s="9"/>
+      <c r="B209" s="9"/>
+      <c r="C209" s="14"/>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A210" s="9"/>
+      <c r="B210" s="9"/>
+      <c r="C210" s="14"/>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A211" s="9"/>
+      <c r="B211" s="9"/>
+      <c r="C211" s="14"/>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A212" s="9"/>
+      <c r="B212" s="9"/>
+      <c r="C212" s="14"/>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A213" s="9"/>
+      <c r="B213" s="9"/>
+      <c r="C213" s="14"/>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A214" s="9"/>
+      <c r="B214" s="9"/>
+      <c r="C214" s="14"/>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A215" s="9"/>
+      <c r="B215" s="9"/>
+      <c r="C215" s="14"/>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A216" s="9"/>
+      <c r="B216" s="9"/>
+      <c r="C216" s="14"/>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A217" s="9"/>
+      <c r="B217" s="9"/>
+      <c r="C217" s="14"/>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A218" s="9"/>
+      <c r="B218" s="9"/>
+      <c r="C218" s="14"/>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A219" s="9"/>
+      <c r="B219" s="9"/>
+      <c r="C219" s="14"/>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A220" s="9"/>
+      <c r="B220" s="9"/>
+      <c r="C220" s="14"/>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A221" s="9"/>
+      <c r="B221" s="9"/>
+      <c r="C221" s="14"/>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A222" s="9"/>
+      <c r="B222" s="9"/>
+      <c r="C222" s="14"/>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A223" s="9"/>
+      <c r="B223" s="9"/>
+      <c r="C223" s="14"/>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A224" s="9"/>
+      <c r="B224" s="9"/>
+      <c r="C224" s="14"/>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A225" s="9"/>
+      <c r="B225" s="9"/>
+      <c r="C225" s="14"/>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A226" s="9"/>
+      <c r="B226" s="9"/>
+      <c r="C226" s="14"/>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A227" s="9"/>
+      <c r="B227" s="9"/>
+      <c r="C227" s="14"/>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A228" s="9"/>
+      <c r="B228" s="9"/>
+      <c r="C228" s="14"/>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A229" s="9"/>
+      <c r="B229" s="9"/>
+      <c r="C229" s="14"/>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A230" s="9"/>
+      <c r="B230" s="9"/>
+      <c r="C230" s="14"/>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A231" s="9"/>
+      <c r="B231" s="9"/>
+      <c r="C231" s="14"/>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A232" s="9"/>
+      <c r="B232" s="9"/>
+      <c r="C232" s="14"/>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A233" s="9"/>
+      <c r="B233" s="9"/>
+      <c r="C233" s="14"/>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A234" s="9"/>
+      <c r="B234" s="9"/>
+      <c r="C234" s="14"/>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A235" s="9"/>
+      <c r="B235" s="9"/>
+      <c r="C235" s="14"/>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A236" s="9"/>
+      <c r="B236" s="9"/>
+      <c r="C236" s="14"/>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A237" s="9"/>
+      <c r="B237" s="9"/>
+      <c r="C237" s="14"/>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A238" s="9"/>
+      <c r="B238" s="9"/>
+      <c r="C238" s="14"/>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A239" s="9"/>
+      <c r="B239" s="9"/>
+      <c r="C239" s="14"/>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A240" s="9"/>
+      <c r="B240" s="9"/>
+      <c r="C240" s="14"/>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A241" s="9"/>
+      <c r="B241" s="9"/>
+      <c r="C241" s="14"/>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A242" s="9"/>
+      <c r="B242" s="9"/>
+      <c r="C242" s="14"/>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A243" s="9"/>
+      <c r="B243" s="9"/>
+      <c r="C243" s="14"/>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A244" s="9"/>
+      <c r="B244" s="9"/>
+      <c r="C244" s="14"/>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A245" s="9"/>
+      <c r="B245" s="9"/>
+      <c r="C245" s="14"/>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A246" s="9"/>
+      <c r="B246" s="9"/>
+      <c r="C246" s="14"/>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A247" s="9"/>
+      <c r="B247" s="9"/>
+      <c r="C247" s="14"/>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A248" s="9"/>
+      <c r="B248" s="9"/>
+      <c r="C248" s="14"/>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A249" s="9"/>
+      <c r="B249" s="9"/>
+      <c r="C249" s="14"/>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A250" s="9"/>
+      <c r="B250" s="9"/>
+      <c r="C250" s="14"/>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A251" s="9"/>
+      <c r="B251" s="9"/>
+      <c r="C251" s="14"/>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A252" s="9"/>
+      <c r="B252" s="9"/>
+      <c r="C252" s="14"/>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A253" s="9"/>
+      <c r="B253" s="9"/>
+      <c r="C253" s="14"/>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A254" s="9"/>
+      <c r="B254" s="9"/>
+      <c r="C254" s="14"/>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A255" s="9"/>
+      <c r="B255" s="9"/>
+      <c r="C255" s="14"/>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A256" s="9"/>
+      <c r="B256" s="9"/>
+      <c r="C256" s="14"/>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A257" s="9"/>
+      <c r="B257" s="9"/>
+      <c r="C257" s="14"/>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A258" s="9"/>
+      <c r="B258" s="9"/>
+      <c r="C258" s="14"/>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A259" s="9"/>
+      <c r="B259" s="9"/>
+      <c r="C259" s="14"/>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A260" s="9"/>
+      <c r="B260" s="9"/>
+      <c r="C260" s="14"/>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A261" s="9"/>
+      <c r="B261" s="9"/>
+      <c r="C261" s="14"/>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A262" s="9"/>
+      <c r="B262" s="9"/>
+      <c r="C262" s="14"/>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A263" s="9"/>
+      <c r="B263" s="9"/>
+      <c r="C263" s="14"/>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A264" s="9"/>
+      <c r="B264" s="9"/>
+      <c r="C264" s="14"/>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A265" s="9"/>
+      <c r="B265" s="9"/>
+      <c r="C265" s="14"/>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A266" s="9"/>
+      <c r="B266" s="9"/>
+      <c r="C266" s="14"/>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A267" s="9"/>
+      <c r="B267" s="9"/>
+      <c r="C267" s="14"/>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A268" s="9"/>
+      <c r="B268" s="9"/>
+      <c r="C268" s="14"/>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A269" s="9"/>
+      <c r="B269" s="9"/>
+      <c r="C269" s="14"/>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A270" s="9"/>
+      <c r="B270" s="9"/>
+      <c r="C270" s="14"/>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A271" s="9"/>
+      <c r="B271" s="9"/>
+      <c r="C271" s="14"/>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A272" s="9"/>
+      <c r="B272" s="9"/>
+      <c r="C272" s="14"/>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A273" s="9"/>
+      <c r="B273" s="9"/>
+      <c r="C273" s="14"/>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A274" s="9"/>
+      <c r="B274" s="9"/>
+      <c r="C274" s="14"/>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A275" s="9"/>
+      <c r="B275" s="9"/>
+      <c r="C275" s="14"/>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A276" s="9"/>
+      <c r="B276" s="9"/>
+      <c r="C276" s="14"/>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A277" s="9"/>
+      <c r="B277" s="9"/>
+      <c r="C277" s="14"/>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A278" s="9"/>
+      <c r="B278" s="9"/>
+      <c r="C278" s="14"/>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A279" s="9"/>
+      <c r="B279" s="9"/>
+      <c r="C279" s="14"/>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A280" s="9"/>
+      <c r="B280" s="9"/>
+      <c r="C280" s="14"/>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A281" s="9"/>
+      <c r="B281" s="9"/>
+      <c r="C281" s="14"/>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A282" s="9"/>
+      <c r="B282" s="9"/>
+      <c r="C282" s="14"/>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A283" s="9"/>
+      <c r="B283" s="9"/>
+      <c r="C283" s="14"/>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A284" s="9"/>
+      <c r="B284" s="9"/>
+      <c r="C284" s="14"/>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A285" s="9"/>
+      <c r="B285" s="9"/>
+      <c r="C285" s="14"/>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A286" s="9"/>
+      <c r="B286" s="9"/>
+      <c r="C286" s="14"/>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A287" s="9"/>
+      <c r="B287" s="9"/>
+      <c r="C287" s="14"/>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A288" s="9"/>
+      <c r="B288" s="9"/>
+      <c r="C288" s="14"/>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A289" s="9"/>
+      <c r="B289" s="9"/>
+      <c r="C289" s="14"/>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A290" s="9"/>
+      <c r="B290" s="9"/>
+      <c r="C290" s="14"/>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A291" s="9"/>
+      <c r="B291" s="9"/>
+      <c r="C291" s="14"/>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A292" s="9"/>
+      <c r="B292" s="9"/>
+      <c r="C292" s="14"/>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A293" s="9"/>
+      <c r="B293" s="9"/>
+      <c r="C293" s="14"/>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A294" s="9"/>
+      <c r="B294" s="9"/>
+      <c r="C294" s="14"/>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A295" s="9"/>
+      <c r="B295" s="9"/>
+      <c r="C295" s="14"/>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A296" s="9"/>
+      <c r="B296" s="9"/>
+      <c r="C296" s="14"/>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A297" s="9"/>
+      <c r="B297" s="9"/>
+      <c r="C297" s="14"/>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A298" s="9"/>
+      <c r="B298" s="9"/>
+      <c r="C298" s="14"/>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A299" s="9"/>
+      <c r="B299" s="9"/>
+      <c r="C299" s="14"/>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A300" s="9"/>
+      <c r="B300" s="9"/>
+      <c r="C300" s="14"/>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A301" s="9"/>
+      <c r="B301" s="9"/>
+      <c r="C301" s="14"/>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A302" s="9"/>
+      <c r="B302" s="9"/>
+      <c r="C302" s="14"/>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A303" s="9"/>
+      <c r="B303" s="9"/>
+      <c r="C303" s="14"/>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A304" s="9"/>
+      <c r="B304" s="9"/>
+      <c r="C304" s="14"/>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A305" s="9"/>
+      <c r="B305" s="9"/>
+      <c r="C305" s="14"/>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A306" s="9"/>
+      <c r="B306" s="9"/>
+      <c r="C306" s="14"/>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A307" s="9"/>
+      <c r="B307" s="9"/>
+      <c r="C307" s="14"/>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A308" s="9"/>
+      <c r="B308" s="9"/>
+      <c r="C308" s="14"/>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A309" s="9"/>
+      <c r="B309" s="9"/>
+      <c r="C309" s="14"/>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A310" s="9"/>
+      <c r="B310" s="9"/>
+      <c r="C310" s="14"/>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A311" s="9"/>
+      <c r="B311" s="9"/>
+      <c r="C311" s="14"/>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A312" s="9"/>
+      <c r="B312" s="9"/>
+      <c r="C312" s="14"/>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A313" s="9"/>
+      <c r="B313" s="9"/>
+      <c r="C313" s="14"/>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A314" s="9"/>
+      <c r="B314" s="9"/>
+      <c r="C314" s="14"/>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A315" s="9"/>
+      <c r="B315" s="9"/>
+      <c r="C315" s="14"/>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A316" s="9"/>
+      <c r="B316" s="9"/>
+      <c r="C316" s="14"/>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A317" s="9"/>
+      <c r="B317" s="9"/>
+      <c r="C317" s="14"/>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A318" s="9"/>
+      <c r="B318" s="9"/>
+      <c r="C318" s="14"/>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A319" s="9"/>
+      <c r="B319" s="9"/>
+      <c r="C319" s="14"/>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A320" s="9"/>
+      <c r="B320" s="9"/>
+      <c r="C320" s="14"/>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A321" s="9"/>
+      <c r="B321" s="9"/>
+      <c r="C321" s="14"/>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A322" s="9"/>
+      <c r="B322" s="9"/>
+      <c r="C322" s="14"/>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A323" s="9"/>
+      <c r="B323" s="9"/>
+      <c r="C323" s="14"/>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A324" s="9"/>
+      <c r="B324" s="9"/>
+      <c r="C324" s="14"/>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A325" s="9"/>
+      <c r="B325" s="9"/>
+      <c r="C325" s="14"/>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A326" s="9"/>
+      <c r="B326" s="9"/>
+      <c r="C326" s="14"/>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A327" s="9"/>
+      <c r="B327" s="9"/>
+      <c r="C327" s="14"/>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A328" s="9"/>
+      <c r="B328" s="9"/>
+      <c r="C328" s="14"/>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A329" s="9"/>
+      <c r="B329" s="9"/>
+      <c r="C329" s="14"/>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A330" s="9"/>
+      <c r="B330" s="9"/>
+      <c r="C330" s="14"/>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A331" s="9"/>
+      <c r="B331" s="9"/>
+      <c r="C331" s="14"/>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A332" s="9"/>
+      <c r="B332" s="9"/>
+      <c r="C332" s="14"/>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A333" s="9"/>
+      <c r="B333" s="9"/>
+      <c r="C333" s="14"/>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A334" s="9"/>
+      <c r="B334" s="9"/>
+      <c r="C334" s="14"/>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A335" s="9"/>
+      <c r="B335" s="9"/>
+      <c r="C335" s="14"/>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A336" s="9"/>
+      <c r="B336" s="9"/>
+      <c r="C336" s="14"/>
+    </row>
+    <row r="337" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A337" s="9"/>
+      <c r="B337" s="9"/>
+      <c r="C337" s="14"/>
+    </row>
+    <row r="338" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A338" s="9"/>
+      <c r="B338" s="9"/>
+      <c r="C338" s="14"/>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A339" s="9"/>
+      <c r="B339" s="9"/>
+      <c r="C339" s="14"/>
+    </row>
+    <row r="340" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A340" s="9"/>
+      <c r="B340" s="9"/>
+      <c r="C340" s="14"/>
+    </row>
+    <row r="341" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A341" s="9"/>
+      <c r="B341" s="9"/>
+      <c r="C341" s="14"/>
+    </row>
+    <row r="342" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A342" s="9"/>
+      <c r="B342" s="9"/>
+      <c r="C342" s="14"/>
+    </row>
+    <row r="343" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A343" s="9"/>
+      <c r="B343" s="9"/>
+      <c r="C343" s="14"/>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A344" s="9"/>
+      <c r="B344" s="9"/>
+      <c r="C344" s="14"/>
+    </row>
+    <row r="345" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A345" s="9"/>
+      <c r="B345" s="9"/>
+      <c r="C345" s="14"/>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A346" s="9"/>
+      <c r="B346" s="9"/>
+      <c r="C346" s="14"/>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A347" s="9"/>
+      <c r="B347" s="9"/>
+      <c r="C347" s="14"/>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A348" s="9"/>
+      <c r="B348" s="9"/>
+      <c r="C348" s="14"/>
+    </row>
+    <row r="349" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A349" s="9"/>
+      <c r="B349" s="9"/>
+      <c r="C349" s="14"/>
+    </row>
+    <row r="350" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A350" s="9"/>
+      <c r="B350" s="9"/>
+      <c r="C350" s="14"/>
+    </row>
+    <row r="351" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A351" s="9"/>
+      <c r="B351" s="9"/>
+      <c r="C351" s="14"/>
+    </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C352" s="13"/>
+    </row>
+    <row r="353" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C353" s="13"/>
+    </row>
+    <row r="354" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C354" s="13"/>
+    </row>
+    <row r="355" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C355" s="13"/>
+    </row>
+    <row r="356" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C356" s="13"/>
+    </row>
+    <row r="357" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C357" s="13"/>
+    </row>
+    <row r="358" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C358" s="13"/>
+    </row>
+    <row r="359" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C359" s="13"/>
+    </row>
+    <row r="360" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C360" s="13"/>
+    </row>
+    <row r="361" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C361" s="13"/>
+    </row>
+    <row r="362" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C362" s="13"/>
+    </row>
+    <row r="363" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C363" s="13"/>
+    </row>
+    <row r="364" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C364" s="13"/>
+    </row>
+    <row r="365" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C365" s="13"/>
+    </row>
+    <row r="366" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C366" s="13"/>
+    </row>
+    <row r="367" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C367" s="13"/>
+    </row>
+    <row r="368" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C368" s="13"/>
+    </row>
+    <row r="369" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C369" s="13"/>
+    </row>
+    <row r="370" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C370" s="13"/>
+    </row>
+    <row r="371" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C371" s="13"/>
+    </row>
+    <row r="372" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C372" s="13"/>
+    </row>
+    <row r="373" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C373" s="13"/>
+    </row>
+    <row r="374" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C374" s="13"/>
+    </row>
+    <row r="375" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C375" s="13"/>
+    </row>
+    <row r="376" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C376" s="13"/>
+    </row>
+    <row r="377" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C377" s="13"/>
+    </row>
+    <row r="378" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C378" s="13"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6650F256-3B44-438C-B09D-A5A5EBB93BAD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6152586C-A782-4C8C-BD4A-33A7E12CE8F9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DACC1BB6-B019-40E0-AB58-E33C7A1DD0AE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Vanessas thesis readign. Still the parameter estimation chapter needs to be read
</commit_message>
<xml_diff>
--- a/Bibliography/BibliographyResearch.xlsx
+++ b/Bibliography/BibliographyResearch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\BipedProject\Bibliography\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69AAC9D-A035-4D60-9683-072CF093C3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA4B758-8110-4E70-8225-81525DEE761C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bibliography" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="91">
   <si>
     <t xml:space="preserve">Topic </t>
   </si>
@@ -282,12 +282,114 @@
 13) Max CoT = 0.32
 14) In this book you can also find information about Denise robot</t>
   </si>
+  <si>
+    <t>22.02.01</t>
+  </si>
+  <si>
+    <t>Vanessa F. Hsu Chen</t>
+  </si>
+  <si>
+    <t>Honda ASIMO</t>
+  </si>
+  <si>
+    <t>Frontal plane oscillations</t>
+  </si>
+  <si>
+    <t>Knees</t>
+  </si>
+  <si>
+    <t>Mechansms</t>
+  </si>
+  <si>
+    <t>Used for</t>
+  </si>
+  <si>
+    <t>Rimless Wheel</t>
+  </si>
+  <si>
+    <t>Suction cups</t>
+  </si>
+  <si>
+    <t>The suction cups make the legs lock when  the swing forward, and the through a carefully tuned air valve, eventually release at the right time.</t>
+  </si>
+  <si>
+    <t>Mechanical latch</t>
+  </si>
+  <si>
+    <t>Used for knee locking mechanism</t>
+  </si>
+  <si>
+    <t>Possitves</t>
+  </si>
+  <si>
+    <t>Negatives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clean design that minimizes actuation in the overal robot
+</t>
+  </si>
+  <si>
+    <t>This design requires the foot to go past the straight-legged position
+Inserts an inherently loose knee
+Complicated design</t>
+  </si>
+  <si>
+    <t>Electromagnets</t>
+  </si>
+  <si>
+    <t>Use of electromagnets in order to keep in the knee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Space - force ratio problems
+</t>
+  </si>
+  <si>
+    <t>Electromagnetic clutches</t>
+  </si>
+  <si>
+    <t>Clutches placed on the side of each knee. Use of suction caps to eliminate the signal delay of the clutches.</t>
+  </si>
+  <si>
+    <t>PlastiDip multipurbose rubber</t>
+  </si>
+  <si>
+    <t>Coating, which claims to be flexible, durable and to provide grip</t>
+  </si>
+  <si>
+    <t>Cable rail</t>
+  </si>
+  <si>
+    <t>Used for safety of the robot when falling</t>
+  </si>
+  <si>
+    <t>Infrared Cameras</t>
+  </si>
+  <si>
+    <t>Used for motion capture. The subject has markers with reflective material placed on multiple points</t>
+  </si>
+  <si>
+    <t>Elimination of noisy data. 
+The motion capture system can calibrate the markers real data</t>
+  </si>
+  <si>
+    <t>In this thesis you can find: 
+1) Conservative walking explanation.  Smaller polygon of support leads considerable motion constrain. As a result they have high energy consumption. Comparison with dynamic stability. (Allows the system to have the ground projection of center of mass to leave the support polygon as long as it re-stabilizes again before falling over
+2) Explanation of passive dynamic walking
+3) Uses parameter estimation of a robot build to match the kneed walker
+4) Explanation of online learning controller of Tedrake (Reinforcement learning) ( The control policy is approximated by gradient descent method. Desired behavior is stable motion in the frontal plane)
+5) 1:5 Lower vs Uper leg mass in order the swing leg to bend the knee as it swings
+6) Uses global stability analysis: Basin of attraction
+7) Use of square aluminum tube for the upper leg. Use of Garolite for the lower legs
+8) Knee locking methods study.
+9) Insertion of switches in order to activate - deactivate the knee lock
+10) Use of cameras as motion sensors for the passive robot. Data parsing using matlab and noise filtering</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,13 +421,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -346,12 +461,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -396,8 +512,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1033,6 +1162,187 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>143436</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>161365</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1183342</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2277453</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A44393EE-4489-F290-4465-D968A336D46D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7297271" y="18386612"/>
+          <a:ext cx="1039906" cy="2116088"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>929640</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1225762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E3DC689-C2BC-841B-1188-9780696D69AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8343900" y="1219200"/>
+          <a:ext cx="845820" cy="1088602"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1022863</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>53341</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1603789</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1318261</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C006571A-1BD4-5E2A-5269-2B92F5F4842D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9282943" y="1135381"/>
+          <a:ext cx="580926" cy="1264920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>83821</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>806835</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1089661</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED82884E-B56C-BEDA-7AB0-B5E5A5DFEC88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14706601" y="3093721"/>
+          <a:ext cx="730634" cy="1005840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1301,8 +1611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1471,9 +1781,16 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="13"/>
-      <c r="D10" s="2"/>
+    <row r="10" spans="1:6" ht="348" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" s="13"/>
@@ -1852,10 +2169,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FAA8682-672A-4E95-AC5A-8804F6AFB6B8}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1898,6 +2215,16 @@
         <v>33</v>
       </c>
     </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1908,7 +2235,7 @@
   <dimension ref="A1:E706"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6573,16 +6900,113 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6152586C-A782-4C8C-BD4A-33A7E12CE8F9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="46.44140625" style="18" customWidth="1"/>
+    <col min="5" max="6" width="46.44140625" style="19" customWidth="1"/>
+    <col min="7" max="7" width="38.6640625" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="9"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="16"/>
+      <c r="B2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="1:7" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="97.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6591,7 +7015,7 @@
   <dimension ref="A1:E404"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6631,24 +7055,38 @@
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="12"/>
+    <row r="3" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>84</v>
+      </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>86</v>
+      </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+    <row r="5" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>89</v>
+      </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
     </row>

</xml_diff>

<commit_message>
Read Phillip Chatzitheodorou thesis
</commit_message>
<xml_diff>
--- a/Bibliography/BibliographyResearch.xlsx
+++ b/Bibliography/BibliographyResearch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\BipedProject\Bibliography\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D3D9FE-E355-44D8-9959-046DD3238CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C9E9B6-F535-472D-8948-5749A23EAB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="902" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bibliography" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="103">
   <si>
     <t xml:space="preserve">Topic </t>
   </si>
@@ -283,9 +283,6 @@
 14) In this book you can also find information about Denise robot</t>
   </si>
   <si>
-    <t>22.02.01</t>
-  </si>
-  <si>
     <t>Vanessa F. Hsu Chen</t>
   </si>
   <si>
@@ -385,6 +382,47 @@
 10) Use of cameras as motion sensors for the passive robot. Data parsing using matlab and noise filtering
 11) Parameters estimation using linear least-squares estimator (LLSE) method
 12)  Indentification of problems such as, Mismatch in the position of the outer feet, Delayed knee lock, Hyper - extension of the leg.</t>
+  </si>
+  <si>
+    <t>22.02.03</t>
+  </si>
+  <si>
+    <t>Philip Hatzitheodorou</t>
+  </si>
+  <si>
+    <t>Biped with knees</t>
+  </si>
+  <si>
+    <t>VanessaFHsuChenThesis.pdf</t>
+  </si>
+  <si>
+    <t>Aldebaran Robotic's NAO</t>
+  </si>
+  <si>
+    <t>SAFFiR (Virginia Teck)</t>
+  </si>
+  <si>
+    <t>Rope transmition</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Sandia's WANDERERER</t>
+  </si>
+  <si>
+    <t>Boston Dynamics Atlas</t>
+  </si>
+  <si>
+    <t>LUIGI (Lght Unactuated Imitator for Gait Insights)</t>
+  </si>
+  <si>
+    <t>DexterIII</t>
+  </si>
+  <si>
+    <t>In this thesis you can find:
+1)  Luigi's upper thigs are divided into cap and body. Use of abs for implementation
+2) Pattela and shank into one peace.</t>
   </si>
 </sst>
 </file>
@@ -1340,6 +1378,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>625301</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>986118</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B99C996E-ECDD-CFB2-6272-A035E09A2E6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7153836" y="23442707"/>
+          <a:ext cx="625300" cy="986117"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>708212</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1362636</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1037200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37B6074C-3127-B69A-DEF9-230F162FF864}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7960659" y="23442706"/>
+          <a:ext cx="654424" cy="1037200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1469,6 +1595,50 @@
         <a:xfrm>
           <a:off x="14706601" y="3093721"/>
           <a:ext cx="730634" cy="1005840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>53788</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>35859</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1177461</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>968188</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7557D18-0FD1-3AD3-73E1-2FC91E1F4983}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14666259" y="4285130"/>
+          <a:ext cx="1123673" cy="932329"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1745,8 +1915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1754,7 +1924,7 @@
     <col min="1" max="1" width="30.88671875" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.21875" style="5" customWidth="1"/>
     <col min="3" max="3" width="39.21875" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" customWidth="1"/>
     <col min="5" max="5" width="54.77734375" style="10" customWidth="1"/>
     <col min="6" max="6" width="30.77734375" style="9" bestFit="1" customWidth="1"/>
   </cols>
@@ -1916,19 +2086,32 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="B10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="F10" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C11" s="13"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" s="13"/>
@@ -2294,24 +2477,25 @@
     <hyperlink ref="F7" r:id="rId6" display="Consept/NoKnees/Vasileiou_Thesis_2019.pdf" xr:uid="{42DB3B71-B4CF-498E-A846-5EACFC5F9B67}"/>
     <hyperlink ref="F8" r:id="rId7" display="Manufacturers/CollinsRuinaPassiveLegsKnees.pdf" xr:uid="{E03437DA-8456-4E3D-A8B2-249AE9844B57}"/>
     <hyperlink ref="F9" r:id="rId8" display="Manufacturers/WisseBookMikeDesign.pdf" xr:uid="{6C7A0374-5A96-4F7A-A122-2AA6BCDAE8E4}"/>
+    <hyperlink ref="F10" r:id="rId9" display="Manufacturers/VanessaFHsuChenThesis.pdf" xr:uid="{FA22FBAE-4BC2-4EED-88B6-8494A8D03E65}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId9"/>
-  <drawing r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId10"/>
+  <drawing r:id="rId11"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FAA8682-672A-4E95-AC5A-8804F6AFB6B8}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.88671875" customWidth="1"/>
+    <col min="1" max="1" width="48.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -2351,12 +2535,42 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -7034,10 +7248,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6152586C-A782-4C8C-BD4A-33A7E12CE8F9}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="C5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7053,20 +7267,20 @@
   <sheetData>
     <row r="1" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>67</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>68</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19" t="s">
         <v>45</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>74</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>75</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>4</v>
@@ -7075,10 +7289,10 @@
     <row r="2" spans="1:7" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19"/>
       <c r="B2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
@@ -7087,47 +7301,56 @@
     </row>
     <row r="3" spans="1:7" ht="43.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>76</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>79</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="97.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="E7" s="18" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -7191,10 +7414,10 @@
     </row>
     <row r="3" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>84</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -7202,10 +7425,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>85</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>86</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -7213,13 +7436,13 @@
     </row>
     <row r="5" spans="1:5" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="C5" s="12" t="s">
         <v>88</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>89</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>

</xml_diff>